<commit_message>
Updated excel, readme, and added gitignore
</commit_message>
<xml_diff>
--- a/My Excel.xlsx
+++ b/My Excel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Desktop\testDataViz\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Desktop\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53AFAAA-9790-4115-A515-0019B375DEA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52BB1AF9-616B-450C-89B7-BD24461F9242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="1035" windowWidth="33495" windowHeight="14565" xr2:uid="{3D857BCF-1A92-4370-B4EB-D89201E8A162}"/>
+    <workbookView xWindow="-26460" yWindow="270" windowWidth="22455" windowHeight="14565" xr2:uid="{3D857BCF-1A92-4370-B4EB-D89201E8A162}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,12 +36,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Be the change you want to see</t>
   </si>
   <si>
     <t>Hello everybody</t>
+  </si>
+  <si>
+    <t>Another phrase</t>
   </si>
 </sst>
 </file>
@@ -413,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65270F37-D862-43BE-B319-5F6D5F699B15}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,6 +434,11 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>